<commit_message>
Support to 2022 events
</commit_message>
<xml_diff>
--- a/region_ranking.xlsx
+++ b/region_ranking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Region</t>
   </si>
@@ -22,12 +22,12 @@
     <t>Overall Score</t>
   </si>
   <si>
+    <t>Korea</t>
+  </si>
+  <si>
     <t>China</t>
   </si>
   <si>
-    <t>Korea</t>
-  </si>
-  <si>
     <t>Europe</t>
   </si>
   <si>
@@ -53,18 +53,6 @@
   </si>
   <si>
     <t>Latin America</t>
-  </si>
-  <si>
-    <t>LAN</t>
-  </si>
-  <si>
-    <t>LMS</t>
-  </si>
-  <si>
-    <t>SEA</t>
-  </si>
-  <si>
-    <t>Vietnam</t>
   </si>
 </sst>
 </file>
@@ -422,7 +410,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -441,7 +429,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -449,7 +437,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -457,7 +445,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -465,7 +453,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -473,7 +461,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -522,38 +510,6 @@
       </c>
       <c r="B12">
         <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>